<commit_message>
added test data file
</commit_message>
<xml_diff>
--- a/com.vikas.testng/TestData/TestData.xlsx
+++ b/com.vikas.testng/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suuresh\git\VikasAutomation\com.vikas.testng\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A859A8-B288-42D7-AC3A-7143AB069D6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD81EDE5-EC8F-4C1C-954A-2552E430F9C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>TestCasesName</t>
   </si>
@@ -67,13 +67,16 @@
   </si>
   <si>
     <t>Kurry</t>
+  </si>
+  <si>
+    <t>Couple honeymoon sex at home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +88,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,14 +124,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,7 +416,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,6 +465,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
@@ -465,7 +482,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" tooltip="Couple honeymoon sex at home" display="https://www.xvideos.com/video48670883/couple_honeymoon_sex_at_home" xr:uid="{5543ED61-E700-4D59-BF2D-24DC0F01C4AE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>